<commit_message>
Correctly apply XLSortOrder sortOrder parameter for table sorting. Fixes #705
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Ranges/Sorting.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Ranges/Sorting.xlsx
@@ -7,23 +7,24 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Table" sheetId="2" r:id="rId2"/>
-    <x:sheet name="Rows" sheetId="3" r:id="rId3"/>
-    <x:sheet name="Columns" sheetId="4" r:id="rId4"/>
-    <x:sheet name="Mixed" sheetId="5" r:id="rId5"/>
-    <x:sheet name="Numbers" sheetId="6" r:id="rId6"/>
-    <x:sheet name="TimeSpans" sheetId="7" r:id="rId7"/>
-    <x:sheet name="Dates" sheetId="8" r:id="rId8"/>
-    <x:sheet name="Include Blanks" sheetId="9" r:id="rId9"/>
-    <x:sheet name="Include Blanks Column" sheetId="10" r:id="rId10"/>
-    <x:sheet name="Include Blanks Column Desc" sheetId="11" r:id="rId11"/>
-    <x:sheet name="Case Sensitive" sheetId="12" r:id="rId12"/>
-    <x:sheet name="Case Sensitive Column" sheetId="13" r:id="rId13"/>
-    <x:sheet name="Case Sensitive Column Desc" sheetId="14" r:id="rId14"/>
-    <x:sheet name="Simple" sheetId="15" r:id="rId15"/>
-    <x:sheet name="Simple Desc" sheetId="16" r:id="rId16"/>
-    <x:sheet name="Simple Columns" sheetId="17" r:id="rId17"/>
-    <x:sheet name="Simple Column" sheetId="18" r:id="rId18"/>
-    <x:sheet name="Simple Column Desc" sheetId="19" r:id="rId19"/>
+    <x:sheet name="Table2" sheetId="3" r:id="rId3"/>
+    <x:sheet name="Rows" sheetId="4" r:id="rId4"/>
+    <x:sheet name="Columns" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Mixed" sheetId="6" r:id="rId6"/>
+    <x:sheet name="Numbers" sheetId="7" r:id="rId7"/>
+    <x:sheet name="TimeSpans" sheetId="8" r:id="rId8"/>
+    <x:sheet name="Dates" sheetId="9" r:id="rId9"/>
+    <x:sheet name="Include Blanks" sheetId="10" r:id="rId10"/>
+    <x:sheet name="Include Blanks Column" sheetId="11" r:id="rId11"/>
+    <x:sheet name="Include Blanks Column Desc" sheetId="12" r:id="rId12"/>
+    <x:sheet name="Case Sensitive" sheetId="13" r:id="rId13"/>
+    <x:sheet name="Case Sensitive Column" sheetId="14" r:id="rId14"/>
+    <x:sheet name="Case Sensitive Column Desc" sheetId="15" r:id="rId15"/>
+    <x:sheet name="Simple" sheetId="16" r:id="rId16"/>
+    <x:sheet name="Simple Desc" sheetId="17" r:id="rId17"/>
+    <x:sheet name="Simple Columns" sheetId="18" r:id="rId18"/>
+    <x:sheet name="Simple Column" sheetId="19" r:id="rId19"/>
+    <x:sheet name="Simple Column Desc" sheetId="20" r:id="rId20"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -706,40 +707,40 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:1">
-      <x:c r="A1" s="3" t="s">
+      <x:c r="A1" s="2" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:1">
+      <x:c r="A2" s="6" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:1">
+      <x:c r="A3" s="8" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:1">
+      <x:c r="A4" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:1">
+      <x:c r="A5" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:1">
+      <x:c r="A6" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:1">
+      <x:c r="A7" s="7" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:1">
+      <x:c r="A8" s="3" t="s">
         <x:v>7</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:1">
-      <x:c r="A2" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:1">
-      <x:c r="A3" s="7" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:1">
-      <x:c r="A4" s="5" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:1">
-      <x:c r="A5" s="4" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:1">
-      <x:c r="A6" s="8" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:1">
-      <x:c r="A7" s="2" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:1">
-      <x:c r="A8" s="6" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -751,162 +752,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:C8"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:3">
-      <x:c r="A1" s="8" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B1" s="8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C1" s="8" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:3">
-      <x:c r="A2" s="7" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B2" s="7" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C2" s="7" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3">
-      <x:c r="A3" s="5" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B3" s="5" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C3" s="5" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
-      <x:c r="A4" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B4" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C4" s="6" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3">
-      <x:c r="A5" s="4" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B5" s="4" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C5" s="4" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:3">
-      <x:c r="A6" s="3" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B6" s="3" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C6" s="3" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:3">
-      <x:c r="A7" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B7" s="1" t="s"/>
-      <x:c r="C7" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3">
-      <x:c r="A8" s="2" t="s"/>
-      <x:c r="B8" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C8" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:A8"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:1">
-      <x:c r="A1" s="8" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:1">
-      <x:c r="A2" s="4" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:1">
-      <x:c r="A3" s="5" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:1">
-      <x:c r="A4" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:1">
-      <x:c r="A5" s="7" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:1">
-      <x:c r="A6" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:1">
-      <x:c r="A7" s="6" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:1">
-      <x:c r="A8" s="2" t="s"/>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -962,7 +807,219 @@
 </x:worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C8"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="8" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B1" s="8" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C1" s="8" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C2" s="7" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B3" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C3" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C4" s="6" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B5" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C5" s="4" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B6" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C6" s="3" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:3">
+      <x:c r="A7" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B7" s="1" t="s"/>
+      <x:c r="C7" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3">
+      <x:c r="A8" s="2" t="s"/>
+      <x:c r="B8" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A8"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" s="8" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:1">
+      <x:c r="A2" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:1">
+      <x:c r="A3" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:1">
+      <x:c r="A4" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:1">
+      <x:c r="A5" s="7" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:1">
+      <x:c r="A6" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:1">
+      <x:c r="A7" s="6" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:1">
+      <x:c r="A8" s="2" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A8"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:1">
+      <x:c r="A2" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:1">
+      <x:c r="A3" s="7" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:1">
+      <x:c r="A4" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:1">
+      <x:c r="A5" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:1">
+      <x:c r="A6" s="8" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:1">
+      <x:c r="A7" s="2" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:1">
+      <x:c r="A8" s="6" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1043,106 +1100,6 @@
       <x:c r="C7" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3">
-      <x:c r="A8" s="2" t="s"/>
-      <x:c r="B8" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C8" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:C8"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:3">
-      <x:c r="A1" s="3" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B1" s="3" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C1" s="3" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:3">
-      <x:c r="A2" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B2" s="1" t="s"/>
-      <x:c r="C2" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3">
-      <x:c r="A3" s="8" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B3" s="8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C3" s="8" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
-      <x:c r="A4" s="5" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B4" s="5" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C4" s="5" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3">
-      <x:c r="A5" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B5" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C5" s="6" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3">
-      <x:c r="A6" s="7" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B6" s="7" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C6" s="7" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:3">
-      <x:c r="A7" s="4" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B7" s="4" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C7" s="4" t="s"/>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="2" t="s"/>
@@ -1183,24 +1140,22 @@
       <x:c r="C1" s="3" t="s"/>
     </x:row>
     <x:row r="2" spans="1:3">
-      <x:c r="A2" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B2" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C2" s="6" t="s">
-        <x:v>3</x:v>
+      <x:c r="A2" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s"/>
+      <x:c r="C2" s="1" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
-      <x:c r="A3" s="7" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B3" s="7" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C3" s="7" t="s">
+      <x:c r="A3" s="8" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B3" s="8" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
@@ -1216,40 +1171,42 @@
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
-      <x:c r="A5" s="4" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B5" s="4" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C5" s="4" t="s"/>
+      <x:c r="A5" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B5" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C5" s="6" t="s">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
-      <x:c r="A6" s="2" t="s"/>
-      <x:c r="B6" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C6" s="2" t="s">
+      <x:c r="A6" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B6" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C6" s="7" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
-      <x:c r="A7" s="8" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B7" s="8" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C7" s="8" t="s">
-        <x:v>5</x:v>
-      </x:c>
+      <x:c r="A7" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B7" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C7" s="4" t="s"/>
     </x:row>
     <x:row r="8" spans="1:3">
-      <x:c r="A8" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B8" s="1" t="s"/>
-      <x:c r="C8" s="1" t="s">
+      <x:c r="A8" s="2" t="s"/>
+      <x:c r="B8" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
@@ -1263,6 +1220,106 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C8"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B1" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C1" s="3" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B2" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C2" s="6" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B3" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C3" s="7" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C4" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B5" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C5" s="4" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="2" t="s"/>
+      <x:c r="B6" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3">
+      <x:c r="A7" s="8" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B7" s="8" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C7" s="8" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3">
+      <x:c r="A8" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B8" s="1" t="s"/>
+      <x:c r="C8" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1318,7 +1375,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1379,6 +1436,120 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
+  <x:dimension ref="A1:C9"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="3" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="8" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" s="8" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="8" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B3" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C3" s="4" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B4" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C4" s="3" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B5" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C5" s="6" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="2" t="s"/>
+      <x:c r="B6" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3">
+      <x:c r="A7" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B7" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C7" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3">
+      <x:c r="A8" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B8" s="7" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C8" s="7" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3">
+      <x:c r="A9" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B9" s="1" t="s"/>
+      <x:c r="C9" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
   <x:dimension ref="A1:C8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
@@ -1412,7 +1583,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1495,7 +1666,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1551,7 +1722,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1607,7 +1778,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1663,7 +1834,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1719,7 +1890,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1817,60 +1988,4 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:A8"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:1">
-      <x:c r="A1" s="2" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:1">
-      <x:c r="A2" s="6" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:1">
-      <x:c r="A3" s="8" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:1">
-      <x:c r="A4" s="4" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:1">
-      <x:c r="A5" s="5" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:1">
-      <x:c r="A6" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:1">
-      <x:c r="A7" s="7" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:1">
-      <x:c r="A8" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Update reference files (worksheet dimensions updated)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Ranges/Sorting.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Ranges/Sorting.xlsx
@@ -1550,7 +1550,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C8"/>
+  <x:dimension ref="A1:C2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1588,7 +1588,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C8"/>
+  <x:dimension ref="A1:B8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>

</xml_diff>